<commit_message>
bug removed related to last commit
</commit_message>
<xml_diff>
--- a/payment.xlsx
+++ b/payment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1514">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -4125,6 +4125,438 @@
   </si>
   <si>
     <t>Wed Jan 24 10:21:55 IST 2018</t>
+  </si>
+  <si>
+    <t>Dibyanshu Shekhar Singh</t>
+  </si>
+  <si>
+    <t>dibyanshusingh7618@gmail.com</t>
+  </si>
+  <si>
+    <t>TX12315</t>
+  </si>
+  <si>
+    <t>GKRP7A8</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 11:07:42 IST 2018</t>
+  </si>
+  <si>
+    <t>shubhamsingh20061997@gmail.com</t>
+  </si>
+  <si>
+    <t>TX13244</t>
+  </si>
+  <si>
+    <t>79AMJQZ</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 11:30:12 IST 2018</t>
+  </si>
+  <si>
+    <t>Rohit Hirania</t>
+  </si>
+  <si>
+    <t>rohithirania@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14791</t>
+  </si>
+  <si>
+    <t>C9CPU8B</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 14:37:43 IST 2018</t>
+  </si>
+  <si>
+    <t>aditya ahuja</t>
+  </si>
+  <si>
+    <t>adityaahuja338@gmail.com</t>
+  </si>
+  <si>
+    <t>TX15012</t>
+  </si>
+  <si>
+    <t>GZUBA3U</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 14:42:31 IST 2018</t>
+  </si>
+  <si>
+    <t>Praveen</t>
+  </si>
+  <si>
+    <t>praveenhonavar45@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14568</t>
+  </si>
+  <si>
+    <t>YXE629B</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 14:44:33 IST 2018</t>
+  </si>
+  <si>
+    <t>Kavya</t>
+  </si>
+  <si>
+    <t>kav.amn.pai@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14600</t>
+  </si>
+  <si>
+    <t>D5KUU29</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 14:51:47 IST 2018</t>
+  </si>
+  <si>
+    <t>Prajna C</t>
+  </si>
+  <si>
+    <t>prajnac20@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14068</t>
+  </si>
+  <si>
+    <t>3HTFQZ4</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 14:53:44 IST 2018</t>
+  </si>
+  <si>
+    <t>Ankita Sharma</t>
+  </si>
+  <si>
+    <t>sharmaankita0031996@gmail.com</t>
+  </si>
+  <si>
+    <t>TX15018</t>
+  </si>
+  <si>
+    <t>SBFC2UB</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 14:54:39 IST 2018</t>
+  </si>
+  <si>
+    <t>Srajan</t>
+  </si>
+  <si>
+    <t>srajankulal.salian@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14591</t>
+  </si>
+  <si>
+    <t>8HEB4RV</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 15:12:26 IST 2018</t>
+  </si>
+  <si>
+    <t>Shreedeeksha CH</t>
+  </si>
+  <si>
+    <t>deekshach99@gmail.com</t>
+  </si>
+  <si>
+    <t>TX11618</t>
+  </si>
+  <si>
+    <t>6BSXMQJ</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 17:41:05 IST 2018</t>
+  </si>
+  <si>
+    <t>DEEPT MURTI MADHAV</t>
+  </si>
+  <si>
+    <t>Deepmadhav2111@gmail.com</t>
+  </si>
+  <si>
+    <t>TX11861</t>
+  </si>
+  <si>
+    <t>VT4MKEB</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 18:53:25 IST 2018</t>
+  </si>
+  <si>
+    <t>POOJA SINGH</t>
+  </si>
+  <si>
+    <t>poojasinghgorakhpur@gmail.com</t>
+  </si>
+  <si>
+    <t>TX11614</t>
+  </si>
+  <si>
+    <t>G2GJ8BE</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 19:16:05 IST 2018</t>
+  </si>
+  <si>
+    <t>SUBRAMANYA R</t>
+  </si>
+  <si>
+    <t>subbu.r2199@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14653</t>
+  </si>
+  <si>
+    <t>37X862Z</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 19:18:20 IST 2018</t>
+  </si>
+  <si>
+    <t>Mayur Singh</t>
+  </si>
+  <si>
+    <t>mayursingh0007@gmail.com</t>
+  </si>
+  <si>
+    <t>TX13787</t>
+  </si>
+  <si>
+    <t>ZQBUGQP</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 19:37:31 IST 2018</t>
+  </si>
+  <si>
+    <t>abhishek srivastava</t>
+  </si>
+  <si>
+    <t>abhisheksrivastava94530@gmail.com</t>
+  </si>
+  <si>
+    <t>TX13807</t>
+  </si>
+  <si>
+    <t>GKA7AVX</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 20:03:01 IST 2018</t>
+  </si>
+  <si>
+    <t>Richard singh</t>
+  </si>
+  <si>
+    <t>raghuvanshismriti080602@gmail.com</t>
+  </si>
+  <si>
+    <t>TX12733</t>
+  </si>
+  <si>
+    <t>CJU998E</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 20:20:12 IST 2018</t>
+  </si>
+  <si>
+    <t>SAIF AHMAD AGHA</t>
+  </si>
+  <si>
+    <t>saif.999rocks@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14522</t>
+  </si>
+  <si>
+    <t>HH2Z2Z4</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 20:48:30 IST 2018</t>
+  </si>
+  <si>
+    <t>ADARSH SINGH CHAUHAN</t>
+  </si>
+  <si>
+    <t>15cs045@bit.ac.in</t>
+  </si>
+  <si>
+    <t>TX14883</t>
+  </si>
+  <si>
+    <t>4MS7VZK</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 21:30:36 IST 2018</t>
+  </si>
+  <si>
+    <t>Dineshkumar A</t>
+  </si>
+  <si>
+    <t>dinesh11mail@gmail.com</t>
+  </si>
+  <si>
+    <t>TX13587</t>
+  </si>
+  <si>
+    <t>A442P8R</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 21:41:12 IST 2018</t>
+  </si>
+  <si>
+    <t>Vasu D</t>
+  </si>
+  <si>
+    <t>vasumsv131@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14767</t>
+  </si>
+  <si>
+    <t>MEFPAKC</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 21:43:27 IST 2018</t>
+  </si>
+  <si>
+    <t>Vikash Sharma</t>
+  </si>
+  <si>
+    <t>vs57633@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14792</t>
+  </si>
+  <si>
+    <t>DPF48X3</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 21:55:18 IST 2018</t>
+  </si>
+  <si>
+    <t>Mohamed Azharudeen M</t>
+  </si>
+  <si>
+    <t>mohamedazhar6666@gmail.com</t>
+  </si>
+  <si>
+    <t>TX15111</t>
+  </si>
+  <si>
+    <t>JDDKEY7</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 21:56:22 IST 2018</t>
+  </si>
+  <si>
+    <t>MAYANK SINGH KANDARI</t>
+  </si>
+  <si>
+    <t>msinghkandari@gmail.com</t>
+  </si>
+  <si>
+    <t>TX13669</t>
+  </si>
+  <si>
+    <t>QB8MNXK</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 22:13:10 IST 2018</t>
+  </si>
+  <si>
+    <t>ALOK SHUKLA</t>
+  </si>
+  <si>
+    <t>ashershuklaofficial@gmail.com</t>
+  </si>
+  <si>
+    <t>TX15015</t>
+  </si>
+  <si>
+    <t>VQMQSX5</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 22:19:24 IST 2018</t>
+  </si>
+  <si>
+    <t>Anurag Amrit</t>
+  </si>
+  <si>
+    <t>aamrit90@gmail.com</t>
+  </si>
+  <si>
+    <t>TX11453</t>
+  </si>
+  <si>
+    <t>Y2QXCV2</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 22:30:44 IST 2018</t>
+  </si>
+  <si>
+    <t>Aman Sharma</t>
+  </si>
+  <si>
+    <t>15cs002@bit.ac.in</t>
+  </si>
+  <si>
+    <t>TX13999</t>
+  </si>
+  <si>
+    <t>X2KZ33S</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 22:37:46 IST 2018</t>
+  </si>
+  <si>
+    <t>lolugu venkatesh</t>
+  </si>
+  <si>
+    <t>venkateshlolugu9912415652@gmail.com</t>
+  </si>
+  <si>
+    <t>TX14348</t>
+  </si>
+  <si>
+    <t>Q9CVXUY</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 22:58:02 IST 2018</t>
+  </si>
+  <si>
+    <t>Ravi Pratap Maurya</t>
+  </si>
+  <si>
+    <t>bit16it21@bit.ac.in</t>
+  </si>
+  <si>
+    <t>TX15124</t>
+  </si>
+  <si>
+    <t>RC8V3VG</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 23:00:49 IST 2018</t>
+  </si>
+  <si>
+    <t>Hemant Gupta</t>
+  </si>
+  <si>
+    <t>scholar.hemantt@gmail.com</t>
+  </si>
+  <si>
+    <t>TX13666</t>
+  </si>
+  <si>
+    <t>3BY57PX</t>
+  </si>
+  <si>
+    <t>Wed Jan 24 23:49:56 IST 2018</t>
   </si>
 </sst>
 </file>
@@ -4473,7 +4905,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I405"/>
+  <dimension ref="A1:I450"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15418,6 +15850,1221 @@
         <v>1369</v>
       </c>
     </row>
+    <row r="406" spans="1:9">
+      <c r="A406" t="n">
+        <v>404</v>
+      </c>
+      <c r="B406" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C406" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D406" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E406" t="s"/>
+      <c r="F406" t="s">
+        <v>21</v>
+      </c>
+      <c r="G406" t="s">
+        <v>1373</v>
+      </c>
+      <c r="H406" t="n">
+        <v>1175</v>
+      </c>
+      <c r="I406" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="407" spans="1:9">
+      <c r="A407" t="n">
+        <v>405</v>
+      </c>
+      <c r="B407" t="s">
+        <v>457</v>
+      </c>
+      <c r="C407" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D407" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E407" t="s"/>
+      <c r="F407" t="s">
+        <v>18</v>
+      </c>
+      <c r="G407" t="s">
+        <v>1377</v>
+      </c>
+      <c r="H407" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I407" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="408" spans="1:9">
+      <c r="A408" t="n">
+        <v>406</v>
+      </c>
+      <c r="B408" t="s">
+        <v>457</v>
+      </c>
+      <c r="C408" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D408" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E408" t="s"/>
+      <c r="F408" t="s">
+        <v>204</v>
+      </c>
+      <c r="G408" t="s">
+        <v>1377</v>
+      </c>
+      <c r="H408" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I408" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="409" spans="1:9">
+      <c r="A409" t="n">
+        <v>407</v>
+      </c>
+      <c r="B409" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C409" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D409" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E409" t="s"/>
+      <c r="F409" t="s">
+        <v>152</v>
+      </c>
+      <c r="G409" t="s">
+        <v>1382</v>
+      </c>
+      <c r="H409" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I409" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="410" spans="1:9">
+      <c r="A410" t="n">
+        <v>408</v>
+      </c>
+      <c r="B410" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C410" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D410" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E410" t="s"/>
+      <c r="F410" t="s">
+        <v>21</v>
+      </c>
+      <c r="G410" t="s">
+        <v>1382</v>
+      </c>
+      <c r="H410" t="n">
+        <v>1175</v>
+      </c>
+      <c r="I410" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="411" spans="1:9">
+      <c r="A411" t="n">
+        <v>409</v>
+      </c>
+      <c r="B411" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C411" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D411" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E411" t="s"/>
+      <c r="F411" t="s">
+        <v>168</v>
+      </c>
+      <c r="G411" t="s">
+        <v>1387</v>
+      </c>
+      <c r="H411" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I411" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="412" spans="1:9">
+      <c r="A412" t="n">
+        <v>410</v>
+      </c>
+      <c r="B412" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C412" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D412" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E412" t="s"/>
+      <c r="F412" t="s">
+        <v>73</v>
+      </c>
+      <c r="G412" t="s">
+        <v>1387</v>
+      </c>
+      <c r="H412" t="n">
+        <v>1200</v>
+      </c>
+      <c r="I412" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="413" spans="1:9">
+      <c r="A413" t="n">
+        <v>411</v>
+      </c>
+      <c r="B413" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C413" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D413" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E413" t="s"/>
+      <c r="F413" t="s">
+        <v>18</v>
+      </c>
+      <c r="G413" t="s">
+        <v>1392</v>
+      </c>
+      <c r="H413" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I413" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="414" spans="1:9">
+      <c r="A414" t="n">
+        <v>412</v>
+      </c>
+      <c r="B414" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C414" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D414" t="s">
+        <v>1396</v>
+      </c>
+      <c r="E414" t="s"/>
+      <c r="F414" t="s">
+        <v>18</v>
+      </c>
+      <c r="G414" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H414" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I414" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="415" spans="1:9">
+      <c r="A415" t="n">
+        <v>413</v>
+      </c>
+      <c r="B415" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C415" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D415" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E415" t="s"/>
+      <c r="F415" t="s">
+        <v>18</v>
+      </c>
+      <c r="G415" t="s">
+        <v>1402</v>
+      </c>
+      <c r="H415" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I415" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="416" spans="1:9">
+      <c r="A416" t="n">
+        <v>414</v>
+      </c>
+      <c r="B416" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C416" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D416" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E416" t="s"/>
+      <c r="F416" t="s">
+        <v>168</v>
+      </c>
+      <c r="G416" t="s">
+        <v>1407</v>
+      </c>
+      <c r="H416" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I416" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="417" spans="1:9">
+      <c r="A417" t="n">
+        <v>415</v>
+      </c>
+      <c r="B417" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C417" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D417" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E417" t="s"/>
+      <c r="F417" t="s">
+        <v>73</v>
+      </c>
+      <c r="G417" t="s">
+        <v>1407</v>
+      </c>
+      <c r="H417" t="n">
+        <v>1200</v>
+      </c>
+      <c r="I417" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="418" spans="1:9">
+      <c r="A418" t="n">
+        <v>416</v>
+      </c>
+      <c r="B418" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C418" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D418" t="s">
+        <v>1411</v>
+      </c>
+      <c r="E418" t="s"/>
+      <c r="F418" t="s">
+        <v>18</v>
+      </c>
+      <c r="G418" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H418" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I418" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="419" spans="1:9">
+      <c r="A419" t="n">
+        <v>417</v>
+      </c>
+      <c r="B419" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C419" t="s">
+        <v>1415</v>
+      </c>
+      <c r="D419" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E419" t="s"/>
+      <c r="F419" t="s">
+        <v>18</v>
+      </c>
+      <c r="G419" t="s">
+        <v>1417</v>
+      </c>
+      <c r="H419" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I419" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="420" spans="1:9">
+      <c r="A420" t="n">
+        <v>418</v>
+      </c>
+      <c r="B420" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C420" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D420" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E420" t="s"/>
+      <c r="F420" t="s">
+        <v>168</v>
+      </c>
+      <c r="G420" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H420" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I420" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="421" spans="1:9">
+      <c r="A421" t="n">
+        <v>419</v>
+      </c>
+      <c r="B421" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C421" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D421" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E421" t="s"/>
+      <c r="F421" t="s">
+        <v>106</v>
+      </c>
+      <c r="G421" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H421" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I421" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="422" spans="1:9">
+      <c r="A422" t="n">
+        <v>420</v>
+      </c>
+      <c r="B422" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C422" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D422" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E422" t="s"/>
+      <c r="F422" t="s">
+        <v>18</v>
+      </c>
+      <c r="G422" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H422" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I422" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="423" spans="1:9">
+      <c r="A423" t="n">
+        <v>421</v>
+      </c>
+      <c r="B423" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C423" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D423" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E423" t="s"/>
+      <c r="F423" t="s">
+        <v>18</v>
+      </c>
+      <c r="G423" t="s">
+        <v>1432</v>
+      </c>
+      <c r="H423" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I423" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="424" spans="1:9">
+      <c r="A424" t="n">
+        <v>422</v>
+      </c>
+      <c r="B424" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C424" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D424" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E424" t="s"/>
+      <c r="F424" t="s">
+        <v>152</v>
+      </c>
+      <c r="G424" t="s">
+        <v>1437</v>
+      </c>
+      <c r="H424" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I424" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="425" spans="1:9">
+      <c r="A425" t="n">
+        <v>423</v>
+      </c>
+      <c r="B425" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C425" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D425" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E425" t="s"/>
+      <c r="F425" t="s">
+        <v>25</v>
+      </c>
+      <c r="G425" t="s">
+        <v>1437</v>
+      </c>
+      <c r="H425" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I425" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="426" spans="1:9">
+      <c r="A426" t="n">
+        <v>424</v>
+      </c>
+      <c r="B426" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C426" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D426" t="s">
+        <v>1441</v>
+      </c>
+      <c r="E426" t="s"/>
+      <c r="F426" t="s">
+        <v>152</v>
+      </c>
+      <c r="G426" t="s">
+        <v>1442</v>
+      </c>
+      <c r="H426" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I426" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="427" spans="1:9">
+      <c r="A427" t="n">
+        <v>425</v>
+      </c>
+      <c r="B427" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C427" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D427" t="s">
+        <v>1441</v>
+      </c>
+      <c r="E427" t="s"/>
+      <c r="F427" t="s">
+        <v>25</v>
+      </c>
+      <c r="G427" t="s">
+        <v>1442</v>
+      </c>
+      <c r="H427" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I427" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="428" spans="1:9">
+      <c r="A428" t="n">
+        <v>426</v>
+      </c>
+      <c r="B428" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C428" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D428" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E428" t="s"/>
+      <c r="F428" t="s">
+        <v>42</v>
+      </c>
+      <c r="G428" t="s">
+        <v>1447</v>
+      </c>
+      <c r="H428" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I428" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="429" spans="1:9">
+      <c r="A429" t="n">
+        <v>427</v>
+      </c>
+      <c r="B429" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C429" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D429" t="s">
+        <v>1451</v>
+      </c>
+      <c r="E429" t="s"/>
+      <c r="F429" t="s">
+        <v>18</v>
+      </c>
+      <c r="G429" t="s">
+        <v>1452</v>
+      </c>
+      <c r="H429" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I429" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="430" spans="1:9">
+      <c r="A430" t="n">
+        <v>428</v>
+      </c>
+      <c r="B430" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C430" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D430" t="s">
+        <v>1451</v>
+      </c>
+      <c r="E430" t="s"/>
+      <c r="F430" t="s">
+        <v>212</v>
+      </c>
+      <c r="G430" t="s">
+        <v>1452</v>
+      </c>
+      <c r="H430" t="n">
+        <v>1400</v>
+      </c>
+      <c r="I430" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="431" spans="1:9">
+      <c r="A431" t="n">
+        <v>429</v>
+      </c>
+      <c r="B431" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C431" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D431" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E431" t="s"/>
+      <c r="F431" t="s">
+        <v>152</v>
+      </c>
+      <c r="G431" t="s">
+        <v>1457</v>
+      </c>
+      <c r="H431" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I431" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="432" spans="1:9">
+      <c r="A432" t="n">
+        <v>430</v>
+      </c>
+      <c r="B432" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C432" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D432" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E432" t="s"/>
+      <c r="F432" t="s">
+        <v>25</v>
+      </c>
+      <c r="G432" t="s">
+        <v>1457</v>
+      </c>
+      <c r="H432" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I432" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="433" spans="1:9">
+      <c r="A433" t="n">
+        <v>431</v>
+      </c>
+      <c r="B433" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C433" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D433" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E433" t="s"/>
+      <c r="F433" t="s">
+        <v>42</v>
+      </c>
+      <c r="G433" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H433" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I433" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="434" spans="1:9">
+      <c r="A434" t="n">
+        <v>432</v>
+      </c>
+      <c r="B434" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C434" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D434" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E434" t="s"/>
+      <c r="F434" t="s">
+        <v>18</v>
+      </c>
+      <c r="G434" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H434" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I434" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="435" spans="1:9">
+      <c r="A435" t="n">
+        <v>433</v>
+      </c>
+      <c r="B435" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C435" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D435" t="s">
+        <v>1471</v>
+      </c>
+      <c r="E435" t="s"/>
+      <c r="F435" t="s">
+        <v>18</v>
+      </c>
+      <c r="G435" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H435" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I435" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="436" spans="1:9">
+      <c r="A436" t="n">
+        <v>434</v>
+      </c>
+      <c r="B436" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C436" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D436" t="s">
+        <v>1471</v>
+      </c>
+      <c r="E436" t="s"/>
+      <c r="F436" t="s">
+        <v>21</v>
+      </c>
+      <c r="G436" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H436" t="n">
+        <v>1175</v>
+      </c>
+      <c r="I436" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="437" spans="1:9">
+      <c r="A437" t="n">
+        <v>435</v>
+      </c>
+      <c r="B437" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C437" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D437" t="s">
+        <v>1476</v>
+      </c>
+      <c r="E437" t="s"/>
+      <c r="F437" t="s">
+        <v>42</v>
+      </c>
+      <c r="G437" t="s">
+        <v>1477</v>
+      </c>
+      <c r="H437" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I437" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="438" spans="1:9">
+      <c r="A438" t="n">
+        <v>436</v>
+      </c>
+      <c r="B438" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C438" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D438" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E438" t="s"/>
+      <c r="F438" t="s">
+        <v>675</v>
+      </c>
+      <c r="G438" t="s">
+        <v>1482</v>
+      </c>
+      <c r="H438" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I438" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="439" spans="1:9">
+      <c r="A439" t="n">
+        <v>437</v>
+      </c>
+      <c r="B439" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C439" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D439" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E439" t="s"/>
+      <c r="F439" t="s">
+        <v>168</v>
+      </c>
+      <c r="G439" t="s">
+        <v>1482</v>
+      </c>
+      <c r="H439" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I439" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="440" spans="1:9">
+      <c r="A440" t="n">
+        <v>438</v>
+      </c>
+      <c r="B440" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C440" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D440" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E440" t="s"/>
+      <c r="F440" t="s">
+        <v>168</v>
+      </c>
+      <c r="G440" t="s">
+        <v>1487</v>
+      </c>
+      <c r="H440" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I440" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9">
+      <c r="A441" t="n">
+        <v>439</v>
+      </c>
+      <c r="B441" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C441" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D441" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E441" t="s"/>
+      <c r="F441" t="s">
+        <v>32</v>
+      </c>
+      <c r="G441" t="s">
+        <v>1487</v>
+      </c>
+      <c r="H441" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I441" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="442" spans="1:9">
+      <c r="A442" t="n">
+        <v>440</v>
+      </c>
+      <c r="B442" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C442" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D442" t="s">
+        <v>1491</v>
+      </c>
+      <c r="E442" t="s"/>
+      <c r="F442" t="s">
+        <v>152</v>
+      </c>
+      <c r="G442" t="s">
+        <v>1492</v>
+      </c>
+      <c r="H442" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I442" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="443" spans="1:9">
+      <c r="A443" t="n">
+        <v>441</v>
+      </c>
+      <c r="B443" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C443" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D443" t="s">
+        <v>1496</v>
+      </c>
+      <c r="E443" t="s"/>
+      <c r="F443" t="s">
+        <v>152</v>
+      </c>
+      <c r="G443" t="s">
+        <v>1497</v>
+      </c>
+      <c r="H443" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I443" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="444" spans="1:9">
+      <c r="A444" t="n">
+        <v>442</v>
+      </c>
+      <c r="B444" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C444" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D444" t="s">
+        <v>1496</v>
+      </c>
+      <c r="E444" t="s"/>
+      <c r="F444" t="s">
+        <v>25</v>
+      </c>
+      <c r="G444" t="s">
+        <v>1497</v>
+      </c>
+      <c r="H444" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I444" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="445" spans="1:9">
+      <c r="A445" t="n">
+        <v>443</v>
+      </c>
+      <c r="B445" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C445" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D445" t="s">
+        <v>1501</v>
+      </c>
+      <c r="E445" t="s"/>
+      <c r="F445" t="s">
+        <v>152</v>
+      </c>
+      <c r="G445" t="s">
+        <v>1502</v>
+      </c>
+      <c r="H445" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I445" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="446" spans="1:9">
+      <c r="A446" t="n">
+        <v>444</v>
+      </c>
+      <c r="B446" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C446" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D446" t="s">
+        <v>1501</v>
+      </c>
+      <c r="E446" t="s"/>
+      <c r="F446" t="s">
+        <v>106</v>
+      </c>
+      <c r="G446" t="s">
+        <v>1502</v>
+      </c>
+      <c r="H446" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I446" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="447" spans="1:9">
+      <c r="A447" t="n">
+        <v>445</v>
+      </c>
+      <c r="B447" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C447" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D447" t="s">
+        <v>1506</v>
+      </c>
+      <c r="E447" t="s"/>
+      <c r="F447" t="s">
+        <v>152</v>
+      </c>
+      <c r="G447" t="s">
+        <v>1507</v>
+      </c>
+      <c r="H447" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I447" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="448" spans="1:9">
+      <c r="A448" t="n">
+        <v>446</v>
+      </c>
+      <c r="B448" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C448" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D448" t="s">
+        <v>1506</v>
+      </c>
+      <c r="E448" t="s"/>
+      <c r="F448" t="s">
+        <v>32</v>
+      </c>
+      <c r="G448" t="s">
+        <v>1507</v>
+      </c>
+      <c r="H448" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I448" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="449" spans="1:9">
+      <c r="A449" t="n">
+        <v>447</v>
+      </c>
+      <c r="B449" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C449" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D449" t="s">
+        <v>1511</v>
+      </c>
+      <c r="E449" t="s"/>
+      <c r="F449" t="s">
+        <v>212</v>
+      </c>
+      <c r="G449" t="s">
+        <v>1512</v>
+      </c>
+      <c r="H449" t="n">
+        <v>1400</v>
+      </c>
+      <c r="I449" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="450" spans="1:9">
+      <c r="A450" t="n">
+        <v>448</v>
+      </c>
+      <c r="B450" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C450" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D450" t="s">
+        <v>1511</v>
+      </c>
+      <c r="E450" t="s"/>
+      <c r="F450" t="s">
+        <v>168</v>
+      </c>
+      <c r="G450" t="s">
+        <v>1512</v>
+      </c>
+      <c r="H450" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I450" t="s">
+        <v>1513</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>